<commit_message>
saving info about booke guests working
</commit_message>
<xml_diff>
--- a/main/src/main/resources/hotel_data.xlsx
+++ b/main/src/main/resources/hotel_data.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\HotelManager\main\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E64E696-3981-4BDD-BB6B-D03F634132AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56CB7CCF-8B0B-4633-A3E3-BBC1CE816023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45960" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
+    <sheet name="Guest State" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -30,10 +25,10 @@
     <t>Hotel Name</t>
   </si>
   <si>
-    <t>Rooms per floor</t>
-  </si>
-  <si>
-    <t>Floor number</t>
+    <t>Floor Number</t>
+  </si>
+  <si>
+    <t>Rooms Per Floor</t>
   </si>
   <si>
     <t>Podcarpatia</t>
@@ -52,28 +47,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <color indexed="8"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <color indexed="8"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -104,13 +90,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -135,9 +122,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Pakiet Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -145,42 +132,42 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -210,12 +197,29 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -245,9 +249,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Pakiet Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -306,13 +327,6 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -321,6 +335,13 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -385,11 +406,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -400,27 +441,29 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="3" width="22.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.9296875" customWidth="1"/>
+    <col min="2" max="2" width="19.796875" customWidth="1"/>
+    <col min="3" max="3" width="19.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3">
@@ -430,7 +473,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -442,46 +485,46 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>101</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>20</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>102</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>22</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>103</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>24</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>104</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>26</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>5</v>
       </c>
     </row>

</xml_diff>